<commit_message>
udpated code for figures
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/210824_FAMES_pot_LW_pub.xlsx
+++ b/analysis/data/raw_data/210824_FAMES_pot_LW_pub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/GJBpottery/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2465FF09-9A4C-4D46-8F72-3066F80B780C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8B78CF-9283-4F45-9296-51ED865C81D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="27760" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E051E140-E4E6-EA4A-B35E-019129C46E0F}">
   <dimension ref="A1:AS19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="AR8" sqref="AR8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -846,7 +846,7 @@
         <v>8148.4757732938597</v>
       </c>
       <c r="AD4" s="3">
-        <f t="shared" ref="AD4:AD9" si="3" xml:space="preserve"> H4*X4*100/5</f>
+        <f t="shared" ref="AD4:AD8" si="3" xml:space="preserve"> H4*X4*100/5</f>
         <v>306.95347125437581</v>
       </c>
       <c r="AE4" s="3">
@@ -1222,11 +1222,11 @@
         <v>1.6675713241099962E-5</v>
       </c>
       <c r="Y8">
-        <f t="shared" ref="Y5:Y9" si="9" xml:space="preserve"> C8*X8*100/5</f>
+        <f t="shared" ref="Y8" si="9" xml:space="preserve"> C8*X8*100/5</f>
         <v>410.06079131262038</v>
       </c>
       <c r="Z8">
-        <f t="shared" ref="Z5:Z9" si="10">D8*X8*100/5</f>
+        <f t="shared" ref="Z8" si="10">D8*X8*100/5</f>
         <v>97.964812577489951</v>
       </c>
       <c r="AA8" s="3">

</xml_diff>